<commit_message>
invoice dir clear fix
</commit_message>
<xml_diff>
--- a/webapp/template/bill_template.xlsx
+++ b/webapp/template/bill_template.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>Business Name</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Bill Paid for August 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>August Bill  less paid</t>
@@ -175,7 +172,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="15"/>
+        <color indexed="23"/>
         <rFont val="Arial"/>
       </rPr>
       <t>https://www.vertex42.com/ExcelTemplates/rental-billing-statement.html</t>
@@ -201,7 +198,7 @@
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="15"/>
+        <color indexed="23"/>
         <rFont val="Arial"/>
       </rPr>
       <t>https://www.vertex42.com/licensing/EULA_privateuse.html</t>
@@ -224,7 +221,7 @@
     <numFmt numFmtId="63" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="64" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -269,20 +266,10 @@
       <name val="Trebuchet MS"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="14"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Trebuchet MS"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="15"/>
-      <name val="Arial"/>
     </font>
     <font>
       <b val="1"/>
@@ -293,12 +280,6 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="9"/>
-      <color indexed="16"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -329,11 +310,6 @@
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Trebuchet MS"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="16"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="11"/>
@@ -373,20 +349,25 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="23"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="15"/>
+      <color indexed="23"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="15"/>
+      <color indexed="23"/>
       <name val="Arial"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="15"/>
+      <color indexed="23"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -405,7 +386,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -417,24 +410,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="21"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="16"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="44">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -500,20 +481,13 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="14"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -557,15 +531,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="8"/>
       </left>
       <right style="thin">
@@ -580,15 +545,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -598,13 +554,33 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="11"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -613,7 +589,18 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -623,10 +610,10 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -634,10 +621,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,7 +647,7 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
         <color indexed="14"/>
@@ -658,7 +658,20 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
         <color indexed="14"/>
@@ -674,7 +687,7 @@
         <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,7 +698,7 @@
         <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -698,7 +711,7 @@
         <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -706,7 +719,9 @@
       <left style="thin">
         <color indexed="14"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
       <top style="thin">
         <color indexed="14"/>
       </top>
@@ -721,7 +736,7 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -730,14 +745,16 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
       <top style="thin">
         <color indexed="14"/>
       </top>
@@ -811,6 +828,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="11"/>
       </left>
@@ -831,6 +859,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="dotted">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="11"/>
       </left>
@@ -870,7 +933,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
@@ -881,7 +944,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
@@ -891,7 +954,7 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="16"/>
+        <color indexed="22"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -900,7 +963,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="16"/>
+        <color indexed="22"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -911,7 +974,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -927,14 +990,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
@@ -951,122 +1008,110 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="59" fontId="7" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="12" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="59" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="10" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="7" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="61" fontId="7" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="61" fontId="7" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="59" fontId="7" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
@@ -1074,247 +1119,253 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="7" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="7" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="7" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="4" fontId="7" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="4" fontId="19" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="7" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="4" fontId="7" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="60" fontId="11" fillId="5" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="7" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="7" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="6" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="10" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="62" fontId="7" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="4" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="60" fontId="14" fillId="5" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="60" fontId="14" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="7" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="7" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="6" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="12" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="62" fontId="7" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="63" fontId="7" fillId="2" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="63" fontId="7" fillId="2" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="63" fontId="22" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="64" fontId="23" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="63" fontId="18" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="64" fontId="19" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="60" fontId="18" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="46" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="7" borderId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="47" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="49" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="60" fontId="22" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="7" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1325,8 +1376,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="19"/>
-          <bgColor indexed="20"/>
+          <fgColor indexed="17"/>
+          <bgColor indexed="18"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1354,8 +1405,6 @@
       <rgbColor rgb="ff8394c9"/>
       <rgbColor rgb="ff8994b6"/>
       <rgbColor rgb="ff7f7f7f"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ff3464ab"/>
       <rgbColor rgb="ff3b4e87"/>
       <rgbColor rgb="ffd8d8d8"/>
       <rgbColor rgb="00000000"/>
@@ -1363,6 +1412,8 @@
       <rgbColor rgb="ffd7dbe6"/>
       <rgbColor rgb="ff002060"/>
       <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff3464ab"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2506,7 +2557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2518,10 +2569,7 @@
     <col min="4" max="4" width="7.67188" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.1719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.8516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1719" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="35.25" customHeight="1">
@@ -2535,666 +2583,529 @@
       <c r="F1" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="8">
+      <c r="A2" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" ht="14.6" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="A3" t="s" s="6">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="16"/>
-      <c r="E3" t="s" s="17">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="11"/>
+      <c r="E3" t="s" s="12">
         <v>4</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="13">
         <f>TODAY()</f>
         <v>45586</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="15"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" t="s" s="8">
+      <c r="A4" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="16"/>
-      <c r="E4" t="s" s="17">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="11"/>
+      <c r="E4" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="F4" t="s" s="21">
+      <c r="F4" t="s" s="14">
         <v>7</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="15"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="8">
+      <c r="A5" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="22"/>
-      <c r="E5" t="s" s="23">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="15"/>
+      <c r="E5" t="s" s="16">
         <v>9</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="17">
         <f>F21</f>
         <v>0</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="15"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="22"/>
-      <c r="E6" t="s" s="17">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="15"/>
+      <c r="E6" t="s" s="12">
         <v>10</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="20">
         <v>45536</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="15"/>
     </row>
     <row r="7" ht="18" customHeight="1">
-      <c r="A7" t="s" s="29">
+      <c r="A7" t="s" s="21">
         <v>11</v>
       </c>
-      <c r="B7" t="s" s="30">
+      <c r="B7" t="s" s="22">
         <v>12</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="15"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" ht="18" customHeight="1">
-      <c r="A8" s="34"/>
-      <c r="B8" t="s" s="35">
+      <c r="A8" s="27"/>
+      <c r="B8" t="s" s="28">
         <v>13</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="15"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" ht="18" customHeight="1">
-      <c r="A9" s="34"/>
-      <c r="B9" t="s" s="38">
+      <c r="A9" s="27"/>
+      <c r="B9" t="s" s="32">
         <v>14</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="15"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="39"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="15"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" ht="16.6" customHeight="1">
-      <c r="A11" t="s" s="42">
+      <c r="A11" t="s" s="36">
         <v>15</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" t="s" s="44">
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" t="s" s="38">
         <v>16</v>
       </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="15"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="40"/>
     </row>
     <row r="12" ht="18" customHeight="1">
-      <c r="A12" t="s" s="46">
+      <c r="A12" t="s" s="41">
         <v>17</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" t="s" s="48">
+      <c r="B12" s="42"/>
+      <c r="C12" t="s" s="43">
         <v>18</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" t="s" s="50">
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" t="s" s="45">
         <v>19</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="15"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="52">
+      <c r="A13" s="46">
         <f>$F$3</f>
         <v>45586</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" t="s" s="54">
+      <c r="B13" s="47"/>
+      <c r="C13" t="s" s="48">
         <v>20</v>
       </c>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56">
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50">
         <f>E23</f>
         <v>0</v>
       </c>
-      <c r="G13" t="s" s="57">
-        <v>21</v>
-      </c>
-      <c r="H13" s="51"/>
-      <c r="I13" s="15"/>
     </row>
     <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="52">
+      <c r="A14" s="46">
         <f>$F$3</f>
         <v>45586</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" t="s" s="59">
-        <v>22</v>
-      </c>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56">
+      <c r="B14" s="51"/>
+      <c r="C14" t="s" s="52">
+        <v>21</v>
+      </c>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="50">
         <f>E24</f>
         <v>0</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="61"/>
     </row>
     <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="52">
+      <c r="A15" s="46">
         <f>$F$6</f>
         <v>45536</v>
       </c>
-      <c r="B15" s="62"/>
-      <c r="C15" t="s" s="59">
-        <v>23</v>
-      </c>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="56">
+      <c r="B15" s="54"/>
+      <c r="C15" t="s" s="52">
+        <v>22</v>
+      </c>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="50">
         <f>F14*0.05</f>
         <v>0</v>
       </c>
-      <c r="G15" s="60"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="15"/>
     </row>
     <row r="16" ht="15" customHeight="1">
-      <c r="A16" s="52">
+      <c r="A16" s="46">
         <f>$F$6</f>
         <v>45536</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" t="s" s="59">
-        <v>24</v>
-      </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56">
+      <c r="B16" s="47"/>
+      <c r="C16" t="s" s="52">
+        <v>23</v>
+      </c>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="50">
         <v>0</v>
       </c>
-      <c r="G16" s="60"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="15"/>
     </row>
     <row r="17" ht="15" customHeight="1">
-      <c r="A17" s="52">
+      <c r="A17" s="46">
         <f>$F$6</f>
         <v>45536</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" t="s" s="59">
-        <v>25</v>
-      </c>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="56">
+      <c r="B17" s="47"/>
+      <c r="C17" t="s" s="52">
+        <v>24</v>
+      </c>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="50">
         <v>0</v>
       </c>
-      <c r="G17" s="60"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="15"/>
     </row>
     <row r="18" ht="15" customHeight="1">
-      <c r="A18" s="52">
+      <c r="A18" s="46">
         <f>$F$6</f>
         <v>45536</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" t="s" s="59">
-        <v>26</v>
-      </c>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56">
+      <c r="B18" s="47"/>
+      <c r="C18" t="s" s="52">
+        <v>25</v>
+      </c>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="50">
         <v>0</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="15"/>
     </row>
     <row r="19" ht="15" customHeight="1">
-      <c r="A19" s="52">
+      <c r="A19" s="46">
         <f>$F$6</f>
         <v>45536</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" t="s" s="59">
+      <c r="B19" s="47"/>
+      <c r="C19" t="s" s="52">
+        <v>26</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" ht="15" customHeight="1">
+      <c r="A20" s="55"/>
+      <c r="B20" s="56"/>
+      <c r="C20" t="s" s="57">
         <v>27</v>
       </c>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56">
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59">
         <v>0</v>
       </c>
-      <c r="G19" s="60"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" s="64"/>
-      <c r="B20" s="65"/>
-      <c r="C20" t="s" s="66">
+    </row>
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" s="60"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" t="s" s="62">
         <v>28</v>
       </c>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67">
-        <v>0</v>
-      </c>
-      <c r="G20" s="60"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" ht="15" customHeight="1">
-      <c r="A21" s="68"/>
-      <c r="B21" s="69"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" t="s" s="70">
-        <v>29</v>
-      </c>
-      <c r="F21" s="71">
+      <c r="F21" s="63">
         <f>SUM(F14:F20)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="72"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="15"/>
     </row>
     <row r="22" ht="15" customHeight="1">
-      <c r="A22" t="s" s="73">
+      <c r="A22" t="s" s="64">
+        <v>29</v>
+      </c>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="66"/>
+    </row>
+    <row r="23" ht="15" customHeight="1">
+      <c r="A23" s="67"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="68"/>
+    </row>
+    <row r="24" ht="15" customHeight="1">
+      <c r="A24" t="s" s="69">
         <v>30</v>
       </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" ht="15" customHeight="1">
-      <c r="A23" s="77"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="15"/>
-    </row>
-    <row r="24" ht="15" customHeight="1">
-      <c r="A24" t="s" s="79">
+      <c r="B24" s="70"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="72"/>
+    </row>
+    <row r="25" ht="15" customHeight="1">
+      <c r="A25" t="s" s="73">
         <v>31</v>
       </c>
-      <c r="B24" s="80"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="15"/>
-    </row>
-    <row r="25" ht="15" customHeight="1">
-      <c r="A25" t="s" s="82">
+      <c r="B25" t="s" s="74">
         <v>32</v>
       </c>
-      <c r="B25" t="s" s="83">
+      <c r="C25" t="s" s="75">
         <v>33</v>
       </c>
-      <c r="C25" t="s" s="84">
+      <c r="D25" t="s" s="76">
         <v>34</v>
       </c>
-      <c r="D25" t="s" s="85">
+      <c r="E25" t="s" s="77">
         <v>35</v>
       </c>
-      <c r="E25" t="s" s="86">
+      <c r="F25" s="72"/>
+    </row>
+    <row r="26" ht="15" customHeight="1">
+      <c r="A26" s="78"/>
+      <c r="B26" s="79">
+        <v>45474</v>
+      </c>
+      <c r="C26" s="79">
+        <v>45505</v>
+      </c>
+      <c r="D26" s="80"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="72"/>
+    </row>
+    <row r="27" ht="15" customHeight="1">
+      <c r="A27" t="s" s="82">
         <v>36</v>
       </c>
-      <c r="F25" s="40"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="15"/>
-    </row>
-    <row r="26" ht="15" customHeight="1">
-      <c r="A26" s="87"/>
-      <c r="B26" s="88">
-        <v>45474</v>
-      </c>
-      <c r="C26" s="88">
-        <v>45505</v>
-      </c>
-      <c r="D26" s="89"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="15"/>
-    </row>
-    <row r="27" ht="15" customHeight="1">
-      <c r="A27" t="s" s="91">
-        <v>37</v>
-      </c>
-      <c r="B27" s="92">
+      <c r="B27" s="83">
         <v>428900</v>
       </c>
-      <c r="C27" s="92">
+      <c r="C27" s="83">
         <v>431770</v>
       </c>
-      <c r="D27" s="93">
+      <c r="D27" s="84">
         <f>C27-B27</f>
         <v>2870</v>
       </c>
-      <c r="E27" s="94">
+      <c r="E27" s="85">
         <f>(C27-B27)*0.011784+1.5</f>
         <v>35.32008</v>
       </c>
-      <c r="F27" s="40"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="15"/>
+      <c r="F27" s="72"/>
     </row>
     <row r="28" ht="15" customHeight="1">
-      <c r="A28" s="87"/>
-      <c r="B28" s="95"/>
-      <c r="C28" s="95"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="15"/>
+      <c r="A28" s="78"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="72"/>
     </row>
     <row r="29" ht="15" customHeight="1">
-      <c r="A29" s="96"/>
-      <c r="B29" s="97"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="97"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="15"/>
+      <c r="A29" s="87"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="85"/>
+      <c r="F29" s="72"/>
     </row>
     <row r="30" ht="15" customHeight="1">
-      <c r="A30" s="87"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="15"/>
+      <c r="A30" s="78"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="90"/>
     </row>
     <row r="31" ht="15" customHeight="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="15"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="72"/>
     </row>
     <row r="32" ht="15" customHeight="1">
-      <c r="A32" s="26"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="15"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="72"/>
     </row>
     <row r="33" ht="15" customHeight="1">
-      <c r="A33" s="26"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="15"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="72"/>
     </row>
     <row r="34" ht="15" customHeight="1">
-      <c r="A34" s="26"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="15"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="72"/>
     </row>
     <row r="35" ht="15" customHeight="1">
-      <c r="A35" t="s" s="99">
+      <c r="A35" t="s" s="91">
+        <v>37</v>
+      </c>
+      <c r="B35" s="92"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="92"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="93"/>
+    </row>
+    <row r="36" ht="15" customHeight="1">
+      <c r="A36" t="s" s="94">
         <v>38</v>
       </c>
-      <c r="B35" s="100"/>
-      <c r="C35" s="100"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="15"/>
-    </row>
-    <row r="36" ht="15" customHeight="1">
-      <c r="A36" t="s" s="101">
+      <c r="B36" s="95"/>
+      <c r="C36" s="96"/>
+      <c r="D36" s="96"/>
+      <c r="E36" t="s" s="97">
         <v>39</v>
       </c>
-      <c r="B36" s="102"/>
-      <c r="C36" s="103"/>
-      <c r="D36" s="103"/>
-      <c r="E36" t="s" s="104">
-        <v>40</v>
-      </c>
-      <c r="F36" s="105">
+      <c r="F36" s="98">
         <f>F3</f>
         <v>45586</v>
       </c>
-      <c r="G36" s="13"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="15"/>
     </row>
     <row r="37" ht="15" customHeight="1">
-      <c r="A37" t="s" s="8">
+      <c r="A37" t="s" s="6">
         <v>0</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" t="s" s="106">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" t="s" s="99">
+        <v>40</v>
+      </c>
+      <c r="F37" t="s" s="100">
+        <f>F4</f>
         <v>41</v>
       </c>
-      <c r="F37" t="s" s="106">
-        <f>F4</f>
+    </row>
+    <row r="38" ht="15" customHeight="1">
+      <c r="A38" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="101"/>
+    </row>
+    <row r="39" ht="15" customHeight="1">
+      <c r="A39" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" t="s" s="102">
         <v>42</v>
       </c>
-      <c r="G37" s="13"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="15"/>
-    </row>
-    <row r="38" ht="15" customHeight="1">
-      <c r="A38" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="107"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="15"/>
-    </row>
-    <row r="39" ht="15" customHeight="1">
-      <c r="A39" t="s" s="8">
-        <v>3</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" t="s" s="108">
-        <v>43</v>
-      </c>
-      <c r="F39" s="109">
+      <c r="F39" s="103">
         <f>F6</f>
         <v>45536</v>
       </c>
-      <c r="G39" s="25"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="15"/>
     </row>
     <row r="40" ht="15" customHeight="1">
-      <c r="A40" s="77"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" t="s" s="108">
-        <v>44</v>
-      </c>
-      <c r="F40" s="110">
+      <c r="A40" s="67"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" t="s" s="102">
+        <v>43</v>
+      </c>
+      <c r="F40" s="104">
         <f>IF(F21&gt;0,F21,0)</f>
         <v>0</v>
       </c>
-      <c r="G40" s="25"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="15"/>
     </row>
     <row r="41" ht="15" customHeight="1">
-      <c r="A41" t="s" s="8">
+      <c r="A41" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="105"/>
+      <c r="F41" s="106"/>
+    </row>
+    <row r="42" ht="15" customHeight="1">
+      <c r="A42" s="18"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="107"/>
+      <c r="E42" t="s" s="108">
         <v>45</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="112"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="15"/>
-    </row>
-    <row r="42" ht="15" customHeight="1">
-      <c r="A42" s="26"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="113"/>
-      <c r="E42" t="s" s="114">
+      <c r="F42" s="109"/>
+    </row>
+    <row r="43" ht="15" customHeight="1">
+      <c r="A43" t="s" s="6">
         <v>46</v>
       </c>
-      <c r="F42" s="115"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="15"/>
-    </row>
-    <row r="43" ht="15" customHeight="1">
-      <c r="A43" t="s" s="8">
-        <v>47</v>
-      </c>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
-      <c r="F43" s="116"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="15"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="110"/>
     </row>
     <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" s="26"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="15"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="90"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" s="117"/>
-      <c r="B45" s="118"/>
-      <c r="C45" s="118"/>
-      <c r="D45" s="118"/>
-      <c r="E45" s="118"/>
-      <c r="F45" s="118"/>
-      <c r="G45" s="118"/>
-      <c r="H45" s="118"/>
-      <c r="I45" s="119"/>
+      <c r="A45" s="111"/>
+      <c r="B45" s="112"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="112"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="113"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C12:C13">
@@ -3224,165 +3135,165 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="120" customWidth="1"/>
-    <col min="2" max="2" width="62.6719" style="120" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="120" customWidth="1"/>
-    <col min="4" max="5" width="9" style="120" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="120" customWidth="1"/>
+    <col min="1" max="1" width="2.5" style="114" customWidth="1"/>
+    <col min="2" max="2" width="62.6719" style="114" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="114" customWidth="1"/>
+    <col min="4" max="5" width="9" style="114" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="114" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.1" customHeight="1">
-      <c r="A1" s="121"/>
-      <c r="B1" t="s" s="122">
+      <c r="A1" s="115"/>
+      <c r="B1" t="s" s="116">
+        <v>47</v>
+      </c>
+      <c r="C1" s="117"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="119"/>
+    </row>
+    <row r="2" ht="16.5" customHeight="1">
+      <c r="A2" s="120"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="90"/>
+    </row>
+    <row r="3" ht="16.5" customHeight="1">
+      <c r="A3" s="18"/>
+      <c r="B3" t="s" s="123">
         <v>48</v>
       </c>
-      <c r="C1" s="123"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" ht="16.5" customHeight="1">
-      <c r="A2" s="124"/>
-      <c r="B2" s="125"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" ht="16.5" customHeight="1">
-      <c r="A3" s="26"/>
-      <c r="B3" t="s" s="127">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="90"/>
+    </row>
+    <row r="4" ht="14.6" customHeight="1">
+      <c r="A4" s="18"/>
+      <c r="B4" t="s" s="124">
         <v>49</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" ht="14.6" customHeight="1">
-      <c r="A4" s="26"/>
-      <c r="B4" t="s" s="128">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="90"/>
+    </row>
+    <row r="5" ht="16.5" customHeight="1">
+      <c r="A5" s="18"/>
+      <c r="B5" s="125"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="90"/>
+    </row>
+    <row r="6" ht="16.6" customHeight="1">
+      <c r="A6" s="18"/>
+      <c r="B6" t="s" s="126">
         <v>50</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="15"/>
-    </row>
-    <row r="5" ht="16.5" customHeight="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="15"/>
-    </row>
-    <row r="6" ht="16.6" customHeight="1">
-      <c r="A6" s="26"/>
-      <c r="B6" t="s" s="130">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="90"/>
+    </row>
+    <row r="7" ht="16.5" customHeight="1">
+      <c r="A7" s="18"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="90"/>
+    </row>
+    <row r="8" ht="31.5" customHeight="1">
+      <c r="A8" s="18"/>
+      <c r="B8" t="s" s="127">
         <v>51</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" ht="16.5" customHeight="1">
-      <c r="A7" s="26"/>
-      <c r="B7" s="129"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" ht="31.5" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" t="s" s="131">
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="90"/>
+    </row>
+    <row r="9" ht="16.5" customHeight="1">
+      <c r="A9" s="18"/>
+      <c r="B9" s="125"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="90"/>
+    </row>
+    <row r="10" ht="31.5" customHeight="1">
+      <c r="A10" s="18"/>
+      <c r="B10" t="s" s="127">
         <v>52</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" ht="16.5" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" ht="31.5" customHeight="1">
-      <c r="A10" s="26"/>
-      <c r="B10" t="s" s="131">
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="90"/>
+    </row>
+    <row r="11" ht="16.5" customHeight="1">
+      <c r="A11" s="18"/>
+      <c r="B11" s="125"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="90"/>
+    </row>
+    <row r="12" ht="31.5" customHeight="1">
+      <c r="A12" s="18"/>
+      <c r="B12" t="s" s="127">
         <v>53</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" ht="16.5" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="129"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" ht="31.5" customHeight="1">
-      <c r="A12" s="26"/>
-      <c r="B12" t="s" s="131">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="90"/>
+    </row>
+    <row r="13" ht="16.5" customHeight="1">
+      <c r="A13" s="18"/>
+      <c r="B13" s="125"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="90"/>
+    </row>
+    <row r="14" ht="16.6" customHeight="1">
+      <c r="A14" s="18"/>
+      <c r="B14" t="s" s="126">
         <v>54</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" s="26"/>
-      <c r="B13" s="129"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" ht="16.6" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" t="s" s="130">
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="90"/>
+    </row>
+    <row r="15" ht="16.6" customHeight="1">
+      <c r="A15" s="18"/>
+      <c r="B15" t="s" s="128">
         <v>55</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" ht="16.6" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" t="s" s="132">
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="90"/>
+    </row>
+    <row r="16" ht="16.5" customHeight="1">
+      <c r="A16" s="18"/>
+      <c r="B16" s="129"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="90"/>
+    </row>
+    <row r="17" ht="16.6" customHeight="1">
+      <c r="A17" s="18"/>
+      <c r="B17" t="s" s="127">
         <v>56</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" ht="16.5" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="133"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" ht="16.6" customHeight="1">
-      <c r="A17" s="26"/>
-      <c r="B17" t="s" s="131">
-        <v>57</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="15"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="90"/>
     </row>
     <row r="18" ht="16.5" customHeight="1">
-      <c r="A18" s="26"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="15"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="90"/>
     </row>
     <row r="19" ht="16.5" customHeight="1">
-      <c r="A19" s="134"/>
-      <c r="B19" s="118"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="118"/>
-      <c r="E19" s="119"/>
+      <c r="A19" s="130"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="113"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>